<commit_message>
final version one day and hday VaR table results
</commit_message>
<xml_diff>
--- a/Results/seminar_results.xlsx
+++ b/Results/seminar_results.xlsx
@@ -5,21 +5,21 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thani\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thani\Dropbox\R_pc_github\Quant-Finance-Seminar\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523A6B82-2F57-4B1A-9ECD-B0F88AF780FB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376A884F-BBF9-4634-B2CC-165D0251FB9F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6480" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sp" sheetId="3" r:id="rId1"/>
-    <sheet name="rds" sheetId="4" r:id="rId2"/>
-    <sheet name="ing" sheetId="5" r:id="rId3"/>
+    <sheet name="gold" sheetId="5" r:id="rId2"/>
+    <sheet name="rds" sheetId="4" r:id="rId3"/>
     <sheet name="aex" sheetId="7" r:id="rId4"/>
     <sheet name="h_day" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="32">
   <si>
     <t>Cond. GARCH EVT</t>
   </si>
@@ -98,35 +98,48 @@
     <t>G evt sp</t>
   </si>
   <si>
-    <t>G EVT rds</t>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TG EVT rds</t>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EG EVT rds</t>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>G EVT aex</t>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TG EVT aex</t>
+    <t>n</t>
   </si>
   <si>
-    <t>EG evt aex</t>
+    <t>S&amp;P</t>
   </si>
   <si>
-    <t>G EVT ing</t>
+    <t>rds</t>
   </si>
   <si>
-    <t>TG EVT ing</t>
+    <t>aex</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>sqrt h rule</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -151,6 +164,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -169,10 +191,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -193,8 +216,15 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,11 +502,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C711DE18-B86C-4AC0-8094-CFD0C474FBD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" activeCellId="2" sqref="B2 B15 B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -590,13 +620,13 @@
       <c r="B6" s="2">
         <v>383</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="6">
         <v>0.5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="6">
         <v>0.16</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="6">
         <v>0.3</v>
       </c>
       <c r="I6" s="1"/>
@@ -610,13 +640,13 @@
       <c r="B7" s="2">
         <v>367</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="6">
         <v>0.86</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="6">
         <v>0.36</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="6">
         <v>0.65</v>
       </c>
     </row>
@@ -627,13 +657,13 @@
       <c r="B8" s="2">
         <v>366</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="6">
         <v>0.82</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="6">
         <v>0.82</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="6">
         <v>0.95</v>
       </c>
     </row>
@@ -644,13 +674,13 @@
       <c r="B9" s="2">
         <v>405</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="6">
         <v>0.53</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="6">
         <v>0.15</v>
       </c>
     </row>
@@ -661,13 +691,13 @@
       <c r="B10" s="2">
         <v>402</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="6">
         <v>0.1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="6">
         <v>0.79</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="6">
         <v>0.24</v>
       </c>
     </row>
@@ -678,13 +708,13 @@
       <c r="B11" s="2">
         <v>396</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="6">
         <v>0.17</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="6">
         <v>0.85</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="6">
         <v>0.39</v>
       </c>
     </row>
@@ -695,13 +725,13 @@
       <c r="B12" s="2">
         <v>402</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="6">
         <v>0.1</v>
       </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
         <v>0</v>
       </c>
     </row>
@@ -797,13 +827,13 @@
       <c r="B19" s="2">
         <v>108</v>
       </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6">
         <v>0.62</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="6">
         <v>0</v>
       </c>
     </row>
@@ -814,13 +844,13 @@
       <c r="B20" s="2">
         <v>104</v>
       </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6">
         <v>0.68</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="6">
         <v>0</v>
       </c>
     </row>
@@ -831,13 +861,13 @@
       <c r="B21" s="2">
         <v>107</v>
       </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
         <v>0.63</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="6">
         <v>0</v>
       </c>
     </row>
@@ -848,13 +878,13 @@
       <c r="B22" s="2">
         <v>78</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="6">
         <v>0.65</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="6">
         <v>0.85</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="6">
         <v>0.88</v>
       </c>
     </row>
@@ -865,13 +895,13 @@
       <c r="B23" s="2">
         <v>87</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="6">
         <v>0.98</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="6">
         <v>0.34</v>
       </c>
     </row>
@@ -882,13 +912,13 @@
       <c r="B24" s="2">
         <v>89</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="6">
         <v>0.09</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="6">
         <v>0.95</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="6">
         <v>0.24</v>
       </c>
     </row>
@@ -899,13 +929,13 @@
       <c r="B25" s="2">
         <v>85</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="6">
         <v>0.21</v>
       </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1006,13 +1036,13 @@
       <c r="B32" s="2">
         <v>62</v>
       </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="6">
         <v>0</v>
       </c>
       <c r="H32" s="1"/>
@@ -1028,13 +1058,13 @@
       <c r="B33" s="2">
         <v>65</v>
       </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6">
         <v>0.6</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1045,13 +1075,13 @@
       <c r="B34" s="2">
         <v>65</v>
       </c>
-      <c r="C34" s="2">
-        <v>0</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
         <v>0.6</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1062,13 +1092,13 @@
       <c r="B35" s="2">
         <v>45</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="6">
         <v>0.2</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="6">
         <v>0.25</v>
       </c>
     </row>
@@ -1079,13 +1109,13 @@
       <c r="B36" s="2">
         <v>44</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="6">
         <v>0.26</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="6">
         <v>0.27</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="6">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -1096,13 +1126,13 @@
       <c r="B37" s="2">
         <v>47</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="6">
         <v>0.12</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="6">
         <v>0.31</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="6">
         <v>0.17</v>
       </c>
     </row>
@@ -1113,13 +1143,13 @@
       <c r="B38" s="2">
         <v>48</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="6">
         <v>0.08</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="6">
         <v>0.04</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="6">
         <v>0.03</v>
       </c>
     </row>
@@ -1130,11 +1160,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897F0043-52FE-4075-A00E-883E9E131FB6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B28" activeCellId="2" sqref="B2 B15 B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1166,7 +1196,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="2">
-        <v>240</v>
+        <v>539</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1176,54 +1206,53 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
-        <v>247</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.62074743499999996</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.51481169800000004</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.71566249599999998</v>
-      </c>
+      <c r="B3" s="2">
+        <v>523</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.48016734956931895</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.12744603290340806</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.24392070349390638</v>
+      </c>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
-        <v>244</v>
-      </c>
-      <c r="C4">
-        <v>0.76612099300000003</v>
-      </c>
-      <c r="D4">
-        <v>0.116420886</v>
-      </c>
-      <c r="E4">
-        <v>0.27897027299999999</v>
-      </c>
-      <c r="F4" s="3"/>
+      <c r="B4" s="2">
+        <v>536</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.89792906341220857</v>
+      </c>
+      <c r="D4" s="6">
+        <v>7.6816672748614145E-5</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3.9931407648174932E-4</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
-        <v>244</v>
-      </c>
-      <c r="C5">
-        <v>0.76612099300000003</v>
-      </c>
-      <c r="D5">
-        <v>0.116420886</v>
-      </c>
-      <c r="E5">
-        <v>0.27897027299999999</v>
-      </c>
-      <c r="F5" s="3"/>
+      <c r="B5" s="2">
+        <v>532</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.75992972599999997</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2.1664899999999999E-4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1.020843E-3</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1235,35 +1264,34 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>251</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.81</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.73</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="1"/>
+        <v>437</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>245</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.72</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.48</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.73</v>
+        <v>451</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1271,16 +1299,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>246</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.43</v>
+        <v>444</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1288,16 +1316,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>275</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.41</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.05</v>
+        <v>500</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.06</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1305,16 +1333,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>262</v>
-      </c>
-      <c r="C10" s="2">
+        <v>506</v>
+      </c>
+      <c r="C10" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.26</v>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1322,16 +1350,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>281</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.52</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.02</v>
+        <v>522</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.46</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1339,15 +1367,15 @@
         <v>9</v>
       </c>
       <c r="B12" s="2">
-        <v>237</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.87</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
+        <v>516</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1355,7 +1383,6 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
@@ -1376,14 +1403,13 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1391,61 +1417,60 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="3">
-        <v>50</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.76205189100000004</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.55217545499999998</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.80046916899999998</v>
-      </c>
+      <c r="B16" s="2">
+        <v>97</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.28842743448367802</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.29697847156313617</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.3304400045486876</v>
+      </c>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>0.76205189100000004</v>
-      </c>
-      <c r="D17">
-        <v>0.55217545499999998</v>
-      </c>
-      <c r="E17">
-        <v>0.80046916899999998</v>
+      <c r="B17" s="2">
+        <v>103</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.64107621531975467</v>
+      </c>
+      <c r="D17" s="6">
+        <v>9.8151464420878853E-2</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.22847425376976105</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18">
-        <v>50</v>
-      </c>
-      <c r="C18">
-        <v>0.76205189100000004</v>
-      </c>
-      <c r="D18">
-        <v>0.11338269500000001</v>
-      </c>
-      <c r="E18">
-        <v>0.272789752</v>
+      <c r="B18" s="2">
+        <v>106</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.86281504499999995</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.40010901700000001</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.69147531200000001</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1453,15 +1478,15 @@
         <v>3</v>
       </c>
       <c r="B19" s="2">
-        <v>81</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
+        <v>150</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="E19" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1470,15 +1495,15 @@
         <v>4</v>
       </c>
       <c r="B20" s="2">
-        <v>80</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="E20" s="2">
+        <v>162</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="E20" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1487,15 +1512,15 @@
         <v>5</v>
       </c>
       <c r="B21" s="2">
-        <v>82</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E21" s="2">
+        <v>163</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1504,16 +1529,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="2">
-        <v>64</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.88</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.08</v>
+        <v>100</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.47</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1521,16 +1546,16 @@
         <v>7</v>
       </c>
       <c r="B23" s="2">
-        <v>61</v>
-      </c>
-      <c r="C23" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.1</v>
+        <v>111</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.33</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1538,48 +1563,48 @@
         <v>8</v>
       </c>
       <c r="B24" s="2">
-        <v>76</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="E24" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="2">
-        <v>72</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.91</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:12">
+      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
@@ -1597,17 +1622,17 @@
       <c r="E27" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="2">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1617,52 +1642,53 @@
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="3">
-        <v>29</v>
-      </c>
-      <c r="C29" s="3">
-        <v>0.31674299900000003</v>
-      </c>
-      <c r="D29" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E29" s="3" t="e">
-        <v>#N/A</v>
+      <c r="B29" s="2">
+        <v>50</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.59072195366944458</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.23511467518468498</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.4276570922340438</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B30">
-        <v>28</v>
-      </c>
-      <c r="C30">
-        <v>0.41916007799999999</v>
-      </c>
-      <c r="D30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E30" t="e">
-        <v>#N/A</v>
+      <c r="B30" s="2">
+        <v>51</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.69043928526000165</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.24552705360306282</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0.47067211290427513</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B31">
-        <v>27</v>
-      </c>
-      <c r="C31">
-        <v>0.54037049800000003</v>
-      </c>
-      <c r="D31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E31" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="B31" s="2">
+        <v>56</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.77464237899999999</v>
+      </c>
+      <c r="D31" s="6">
+        <v>3.5987627000000001E-2</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.106476444</v>
+      </c>
+      <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12">
@@ -1670,17 +1696,18 @@
         <v>3</v>
       </c>
       <c r="B32" s="2">
-        <v>54</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.376</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:5">
@@ -1688,15 +1715,15 @@
         <v>4</v>
       </c>
       <c r="B33" s="2">
-        <v>53</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E33" s="2">
+        <v>112</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.48</v>
+      </c>
+      <c r="E33" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1705,16 +1732,16 @@
         <v>5</v>
       </c>
       <c r="B34" s="2">
-        <v>53</v>
-      </c>
-      <c r="C34" s="2">
-        <v>0</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>18</v>
+        <v>105</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.39</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1722,16 +1749,16 @@
         <v>6</v>
       </c>
       <c r="B35" s="2">
-        <v>32</v>
-      </c>
-      <c r="C35" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>18</v>
+        <v>49</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.38</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1739,16 +1766,16 @@
         <v>7</v>
       </c>
       <c r="B36" s="2">
-        <v>33</v>
-      </c>
-      <c r="C36" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>18</v>
+        <v>56</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.77</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1756,16 +1783,16 @@
         <v>8</v>
       </c>
       <c r="B37" s="2">
-        <v>42</v>
-      </c>
-      <c r="C37" s="2">
-        <v>0</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.53</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1773,29 +1800,30 @@
         <v>9</v>
       </c>
       <c r="B38" s="2">
-        <v>43</v>
-      </c>
-      <c r="C38" s="2">
-        <v>0</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2">
+        <v>63</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C922746-288F-4E3C-A2ED-62FECE2BBA7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B28" activeCellId="2" sqref="B2 B15 B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1827,7 +1855,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1837,44 +1865,54 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>230</v>
-      </c>
-      <c r="C3">
-        <v>0.52619739399999998</v>
-      </c>
-      <c r="D3">
-        <v>0.737208317</v>
-      </c>
-      <c r="E3">
-        <v>0.77324252900000001</v>
+      <c r="B3" s="5">
+        <v>247</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.62074743499999996</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.51481169800000004</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.71566249599999998</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>232</v>
-      </c>
-      <c r="C4">
-        <v>0.61727968200000005</v>
-      </c>
-      <c r="D4">
-        <v>0.46851153899999998</v>
-      </c>
-      <c r="E4">
-        <v>0.67868583599999999</v>
-      </c>
+      <c r="B4" s="5">
+        <v>244</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.76612099300000003</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.116420886</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0.27897027299999999</v>
+      </c>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="5">
+        <v>244</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.76612099300000003</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.116420886</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.27897027299999999</v>
+      </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1886,60 +1924,69 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>241</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.92</v>
-      </c>
-      <c r="D6" s="2">
+        <v>251</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="E6" s="6">
         <v>0.73</v>
       </c>
-      <c r="E6" s="2">
-        <v>0.94</v>
-      </c>
-      <c r="K6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>233</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.83</v>
+        <v>245</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.48</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.73</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="2">
+        <v>246</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.67</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.43</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>258</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.23</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="E9" s="2">
+        <v>275</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D9" s="6">
         <v>0.41</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1947,49 +1994,57 @@
         <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>248</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.73</v>
+        <v>262</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.47</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.26</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="2">
+        <v>281</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.52</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="2">
-        <v>240</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.98</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
+        <v>237</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.87</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
@@ -2007,10 +2062,10 @@
       <c r="E14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
@@ -2022,73 +2077,81 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16">
-        <v>55</v>
-      </c>
-      <c r="C16">
-        <v>0.31380798599999998</v>
-      </c>
-      <c r="D16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G16" s="2"/>
+      <c r="B16" s="5">
+        <v>50</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.76205189100000004</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.55217545499999998</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.80046916899999998</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17">
-        <v>47</v>
-      </c>
-      <c r="C17">
-        <v>0.89569398300000003</v>
-      </c>
-      <c r="D17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E17" t="e">
-        <v>#N/A</v>
+      <c r="B17" s="2">
+        <v>50</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.76205189100000004</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.55217545499999998</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.80046916899999998</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="B18" s="2">
+        <v>50</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.76205189100000004</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.11338269500000001</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.272789752</v>
+      </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="2">
-        <v>80</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>18</v>
+        <v>81</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -2096,42 +2159,50 @@
         <v>4</v>
       </c>
       <c r="B20" s="2">
-        <v>81</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>18</v>
+        <v>80</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="B21" s="2">
+        <v>82</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="2">
-        <v>65</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>18</v>
+        <v>64</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.08</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2139,57 +2210,65 @@
         <v>7</v>
       </c>
       <c r="B23" s="2">
-        <v>59</v>
-      </c>
-      <c r="C23" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>18</v>
+        <v>61</v>
+      </c>
+      <c r="C23" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.1</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="B24" s="2">
+        <v>76</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="2">
-        <v>66</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
@@ -2207,10 +2286,10 @@
       <c r="E27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
@@ -2227,45 +2306,52 @@
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29">
-        <v>24</v>
-      </c>
-      <c r="C29">
-        <v>0.99183064200000004</v>
-      </c>
-      <c r="D29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E29" t="e">
-        <v>#N/A</v>
+      <c r="B29" s="5">
+        <v>29</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0.31674299900000003</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B30">
-        <v>25</v>
-      </c>
-      <c r="C30">
-        <v>0.83089290199999999</v>
-      </c>
-      <c r="D30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E30" t="e">
-        <v>#N/A</v>
+      <c r="B30" s="2">
+        <v>28</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.41916007799999999</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="K31" s="1"/>
+      <c r="B31" s="2">
+        <v>27</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.54037049800000003</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12">
@@ -2273,18 +2359,17 @@
         <v>3</v>
       </c>
       <c r="B32" s="2">
-        <v>64</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0</v>
+      </c>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:5">
@@ -2292,41 +2377,49 @@
         <v>4</v>
       </c>
       <c r="B33" s="2">
-        <v>54</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>18</v>
+        <v>53</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="B34" s="2">
+        <v>53</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="2">
-        <v>31</v>
-      </c>
-      <c r="C35" s="2">
-        <v>0.17</v>
-      </c>
-      <c r="D35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2335,15 +2428,15 @@
         <v>7</v>
       </c>
       <c r="B36" s="2">
-        <v>27</v>
-      </c>
-      <c r="C36" s="2">
-        <v>0.54</v>
-      </c>
-      <c r="D36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2351,25 +2444,33 @@
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="B37" s="2">
+        <v>42</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="2">
-        <v>33</v>
-      </c>
-      <c r="C38" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2">
+        <v>43</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2379,11 +2480,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B738AF27-1691-4EAD-B708-DFF07AAE56AD}">
-  <dimension ref="A1:L38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B28" activeCellId="2" sqref="B2 B15 B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2426,16 +2527,16 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>248</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>0.62381905800000004</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>0.359587669</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>0.58278641200000003</v>
       </c>
     </row>
@@ -2443,16 +2544,16 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>248</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>0.62381905840876772</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>0.81547371090050413</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>0.86286327206249125</v>
       </c>
     </row>
@@ -2460,16 +2561,16 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>258</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>0.25366170399999999</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>0.81062979599999996</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>0.50650603400000005</v>
       </c>
       <c r="F5" s="3"/>
@@ -2484,16 +2585,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>251</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.81</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.73</v>
+        <v>285</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.01</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -2502,16 +2603,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>245</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.72</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.48</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.73</v>
+        <v>261</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.74</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.39</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2519,16 +2620,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>246</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.43</v>
+        <v>277</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.06</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2536,16 +2637,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>275</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.41</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.05</v>
+        <v>298</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.39</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2553,16 +2654,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>262</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.47</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.26</v>
+        <v>273</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.09</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2570,16 +2671,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>281</v>
-      </c>
-      <c r="C11" s="2">
+        <v>289</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.37</v>
+      </c>
+      <c r="E11" s="6">
         <v>0.01</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.52</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.02</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2587,19 +2688,23 @@
         <v>9</v>
       </c>
       <c r="B12" s="2">
-        <v>237</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.87</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
+        <v>242</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.93</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11">
+      <c r="B13" s="2"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -2612,13 +2717,13 @@
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="2"/>
@@ -2633,9 +2738,9 @@
       <c r="B15" s="2">
         <v>48</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2645,17 +2750,17 @@
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>52</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>0.57795099599999999</v>
       </c>
-      <c r="D16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E16" t="e">
-        <v>#N/A</v>
+      <c r="D16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2666,34 +2771,34 @@
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>56</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>0.26516665432252895</v>
       </c>
-      <c r="D17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E17" t="e">
-        <v>#N/A</v>
+      <c r="D17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>58</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>0.16507680599999999</v>
       </c>
-      <c r="D18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E18" t="e">
-        <v>#N/A</v>
+      <c r="D18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2701,15 +2806,15 @@
         <v>3</v>
       </c>
       <c r="B19" s="2">
-        <v>81</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
+        <v>87</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E19" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2718,15 +2823,15 @@
         <v>4</v>
       </c>
       <c r="B20" s="2">
-        <v>80</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="E20" s="2">
+        <v>82</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="E20" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2735,15 +2840,15 @@
         <v>5</v>
       </c>
       <c r="B21" s="2">
-        <v>82</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E21" s="2">
+        <v>88</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2752,16 +2857,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="2">
-        <v>64</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.88</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.08</v>
+        <v>71</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.01</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2769,16 +2874,16 @@
         <v>7</v>
       </c>
       <c r="B23" s="2">
-        <v>61</v>
-      </c>
-      <c r="C23" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.1</v>
+        <v>68</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2786,15 +2891,15 @@
         <v>8</v>
       </c>
       <c r="B24" s="2">
-        <v>76</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E24" s="2">
+        <v>79</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.78</v>
+      </c>
+      <c r="E24" s="6">
         <v>0</v>
       </c>
       <c r="H24" s="2"/>
@@ -2807,15 +2912,15 @@
         <v>9</v>
       </c>
       <c r="B25" s="2">
-        <v>72</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
+        <v>61</v>
+      </c>
+      <c r="C25" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
         <v>0</v>
       </c>
       <c r="H25" s="2"/>
@@ -2824,6 +2929,10 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:12">
+      <c r="B26" s="2"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2836,13 +2945,13 @@
       <c r="B27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H27" s="2"/>
@@ -2857,59 +2966,59 @@
       <c r="B28" s="2">
         <v>24</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>28</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="6">
         <v>0.43197648199999999</v>
       </c>
-      <c r="D29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E29" t="e">
-        <v>#N/A</v>
+      <c r="D29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>28</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="6">
         <v>0.43197648151580403</v>
       </c>
-      <c r="D30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E30" t="e">
-        <v>#N/A</v>
+      <c r="D30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>33</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>8.3594418000000004E-2</v>
       </c>
-      <c r="D31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E31" t="e">
-        <v>#N/A</v>
+      <c r="D31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="L31" s="1"/>
     </row>
@@ -2918,15 +3027,15 @@
         <v>3</v>
       </c>
       <c r="B32" s="2">
-        <v>54</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="E32" s="2">
+        <v>57</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.19</v>
+      </c>
+      <c r="E32" s="6">
         <v>0</v>
       </c>
       <c r="L32" s="1"/>
@@ -2936,16 +3045,16 @@
         <v>4</v>
       </c>
       <c r="B33" s="2">
-        <v>53</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E33" s="2">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2953,16 +3062,16 @@
         <v>5</v>
       </c>
       <c r="B34" s="2">
-        <v>53</v>
-      </c>
-      <c r="C34" s="2">
-        <v>0</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>18</v>
+        <v>63</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2970,16 +3079,16 @@
         <v>6</v>
       </c>
       <c r="B35" s="2">
-        <v>32</v>
-      </c>
-      <c r="C35" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2987,16 +3096,16 @@
         <v>7</v>
       </c>
       <c r="B36" s="2">
-        <v>33</v>
-      </c>
-      <c r="C36" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3004,16 +3113,16 @@
         <v>8</v>
       </c>
       <c r="B37" s="2">
-        <v>42</v>
-      </c>
-      <c r="C37" s="2">
-        <v>0</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>18</v>
+        <v>48</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3021,17 +3130,23 @@
         <v>9</v>
       </c>
       <c r="B38" s="2">
-        <v>43</v>
-      </c>
-      <c r="C38" s="2">
-        <v>0</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2">
-        <v>0</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3039,301 +3154,632 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87777E13-7C99-4BC3-B68E-F8352628D38B}">
-  <dimension ref="A1:N15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2">
+        <v>370</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <v>241</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2">
+        <v>241</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2">
+        <v>539</v>
+      </c>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" s="2">
+        <v>415</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4.3312574E-2</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="5">
+        <v>235</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.86306933500000005</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2">
+        <v>179</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.48253226399999999</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2">
+        <v>382</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.14669242738933452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" s="5">
+        <v>358</v>
+      </c>
+      <c r="D4" s="7">
+        <v>6.7624584000000001E-2</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <v>196</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.72775942400000004</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2">
+        <v>95</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.47340124608670997</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
+        <v>451</v>
+      </c>
+      <c r="M4" s="6">
+        <v>6.5822905632346718E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C5" s="5">
+        <v>374</v>
+      </c>
+      <c r="D5" s="7">
+        <v>6.8279500000000002E-3</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
+        <v>214</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.84283375699999996</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2">
+        <v>111</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.70697080499999998</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2">
+        <v>552</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.19901892500000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>547</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2.1823653995056702E-12</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
+        <v>261</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1.2692304208405947E-3</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2">
+        <v>173</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.59623134665625477</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2">
+        <v>423</v>
+      </c>
+      <c r="M6" s="6">
+        <v>2.5903149293944883E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2">
+        <v>643</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.15415562569035057</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
+        <v>254</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.28810464993143081</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2">
+        <v>302</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.98665981386393586</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
+        <v>575</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0.59454384808304517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2">
+        <v>74</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
+        <v>48</v>
+      </c>
+      <c r="I10" s="2">
+        <v>48</v>
+      </c>
+      <c r="L10" s="2">
+        <v>108</v>
+      </c>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2">
+        <v>103</v>
+      </c>
+      <c r="D11" s="6">
+        <v>7.3425592999999997E-2</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="5">
+        <v>37</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2">
+        <v>25</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2">
+        <v>36</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="5">
+        <v>100</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.59751638399999996</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2">
+        <v>34</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="2">
+        <v>6</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="2">
+        <v>82</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5">
+        <v>105</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2.1011173000000001E-2</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>39</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2">
+        <v>10</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2">
+        <v>108</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2">
+        <v>225</v>
+      </c>
+      <c r="D14" s="6">
+        <v>6.7242489016683393E-5</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>85</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.65222151825393548</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2">
+        <v>19</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2">
+        <v>129</v>
+      </c>
+      <c r="M14" s="6">
+        <v>0.72330960628535357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2">
+        <v>203</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.21915291644497781</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
+        <v>64</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2">
+        <v>100</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0.3925871379563215</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2">
+        <v>111</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2">
+        <v>37</v>
+      </c>
+      <c r="F18" s="2">
+        <v>24</v>
+      </c>
+      <c r="I18" s="2">
+        <v>24</v>
+      </c>
+      <c r="L18" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2">
+        <v>69</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.67820488099999998</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="5">
+        <v>23</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2">
+        <v>11</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2">
+        <v>13</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5">
+        <v>56</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
+        <v>17</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2">
+        <v>3</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2">
+        <v>40</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="T20" s="2"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5">
+        <v>63</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2">
-        <v>415</v>
-      </c>
-      <c r="B2" s="4">
-        <v>358</v>
-      </c>
-      <c r="C2" s="4">
-        <v>374</v>
-      </c>
-      <c r="E2" s="4">
-        <v>235</v>
-      </c>
-      <c r="F2">
-        <v>196</v>
-      </c>
-      <c r="G2">
-        <v>214</v>
-      </c>
-      <c r="I2">
-        <v>179</v>
-      </c>
-      <c r="J2">
-        <v>95</v>
-      </c>
-      <c r="K2">
-        <v>111</v>
-      </c>
-      <c r="M2">
-        <v>161</v>
-      </c>
-      <c r="N2">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3">
-        <v>4.3312574E-2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>6.7624584000000001E-2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>6.8279500000000002E-3</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.86306933500000005</v>
-      </c>
-      <c r="F3">
-        <v>0.72775942400000004</v>
-      </c>
-      <c r="G3">
-        <v>0.84283375699999996</v>
-      </c>
-      <c r="I3">
-        <v>0.48253226399999999</v>
-      </c>
-      <c r="J3">
-        <v>0.47340124608670997</v>
-      </c>
-      <c r="K3">
-        <v>0.70697080499999998</v>
-      </c>
-      <c r="M3">
-        <v>1.6792983000000001E-2</v>
-      </c>
-      <c r="N3">
-        <v>0.31078492299999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8">
-        <v>103</v>
-      </c>
-      <c r="B8" s="3">
-        <v>100</v>
-      </c>
-      <c r="C8" s="3">
-        <v>105</v>
-      </c>
-      <c r="E8" s="3">
-        <v>37</v>
-      </c>
-      <c r="F8">
-        <v>34</v>
-      </c>
-      <c r="G8">
-        <v>39</v>
-      </c>
-      <c r="I8">
-        <v>25</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
-      </c>
-      <c r="K8">
-        <v>10</v>
-      </c>
-      <c r="M8">
-        <v>20</v>
-      </c>
-      <c r="N8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9">
-        <v>7.3425592999999997E-2</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.59751638399999996</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2.1011173000000001E-2</v>
-      </c>
-      <c r="E9" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N9" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14">
-        <v>69</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="G21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2">
+        <v>4</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2">
+        <v>57</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2">
+        <v>168</v>
+      </c>
+      <c r="D22" s="6">
+        <v>5.413247352514805E-4</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
         <v>56</v>
       </c>
-      <c r="C14" s="3">
-        <v>63</v>
-      </c>
-      <c r="E14" s="3">
-        <v>23</v>
-      </c>
-      <c r="F14">
-        <v>17</v>
-      </c>
-      <c r="G14">
-        <v>22</v>
-      </c>
-      <c r="I14">
-        <v>11</v>
-      </c>
-      <c r="J14">
-        <v>3</v>
-      </c>
-      <c r="K14">
-        <v>4</v>
-      </c>
-      <c r="M14">
-        <v>11</v>
-      </c>
-      <c r="N14">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15">
-        <v>0.67820488099999998</v>
-      </c>
-      <c r="B15" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C15" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E15" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N15" t="e">
-        <v>#N/A</v>
+      <c r="G22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2">
+        <v>13</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2">
+        <v>94</v>
+      </c>
+      <c r="M22" s="6">
+        <v>0.84690702284591701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="2">
+        <v>140</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.66804150851764676</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <v>40</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2">
+        <v>59</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="2">
+        <v>67</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="O28" s="2"/>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="9" t="str">
+        <f>C3 &amp; "  " &amp; "(" &amp; D3 &amp; ")"</f>
+        <v>415  (0.043312574)</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto stash before merge of "fix-data" and "origin/fix-data"
Corrected results
</commit_message>
<xml_diff>
--- a/Results/seminar_results.xlsx
+++ b/Results/seminar_results.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thani\Dropbox\R_pc_github\Quant-Finance-Seminar\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/Repositories/Quant-Finance-Seminar/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376A884F-BBF9-4634-B2CC-165D0251FB9F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6480" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="sp" sheetId="3" r:id="rId1"/>
@@ -19,8 +18,11 @@
     <sheet name="aex" sheetId="7" r:id="rId4"/>
     <sheet name="h_day" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -135,17 +137,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -502,21 +503,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" activeCellId="2" sqref="B2 B15 B28"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="4" max="4" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -533,7 +534,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -544,7 +545,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +562,7 @@
         <v>0.73079455199999999</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -578,7 +579,7 @@
         <v>0.80087837399999995</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -613,7 +614,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -633,7 +634,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -650,7 +651,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -667,7 +668,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -684,7 +685,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -701,7 +702,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -718,7 +719,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -735,13 +736,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -758,7 +759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -769,7 +770,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,7 +787,7 @@
         <v>0.91656326899999996</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -803,7 +804,7 @@
         <v>0.39681062900000003</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -820,7 +821,7 @@
         <v>0.238754719</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -837,7 +838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -854,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -871,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -888,7 +889,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -905,7 +906,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -922,7 +923,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -939,13 +940,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -962,7 +963,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -973,7 +974,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -990,7 +991,7 @@
         <v>0.32949495200000001</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -1007,7 +1008,7 @@
         <v>8.3031912999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -1029,7 +1030,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1052,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -1085,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1136,7 +1137,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -1160,21 +1161,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" activeCellId="2" sqref="B2 B15 B28"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="4" max="4" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1202,7 +1203,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1221,7 @@
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>3.9931407648174932E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1259,7 +1260,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1277,7 +1278,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1294,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1311,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1328,7 +1329,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1345,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1362,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1379,12 +1380,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1404,7 +1405,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1418,7 +1419,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1439,7 +1440,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1456,7 +1457,7 @@
         <v>0.22847425376976105</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -1473,7 +1474,7 @@
         <v>0.69147531200000001</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1490,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1507,7 +1508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +1580,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1600,13 +1601,13 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1627,7 +1628,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1638,7 +1639,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>0.4276570922340438</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>0.47067211290427513</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -1691,7 +1692,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -1710,7 +1711,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -1761,7 +1762,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1778,7 +1779,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -1819,21 +1820,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" activeCellId="2" sqref="B2 B15 B28"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="4" max="4" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1861,7 +1862,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1878,7 +1879,7 @@
         <v>0.71566249599999998</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1896,7 +1897,7 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1919,7 +1920,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1938,7 +1939,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1955,7 +1956,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1972,7 +1973,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1989,7 +1990,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2006,7 +2007,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2023,7 +2024,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2040,13 +2041,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2067,7 +2068,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2082,7 +2083,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2103,7 +2104,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -2120,7 +2121,7 @@
         <v>0.80046916899999998</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>0.272789752</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2154,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2188,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -2222,7 +2223,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -2243,7 +2244,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -2264,13 +2265,13 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -2291,7 +2292,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -2302,7 +2303,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2319,7 +2320,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -2354,7 +2355,7 @@
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -2372,7 +2373,7 @@
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -2389,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -2423,7 +2424,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -2480,21 +2481,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" activeCellId="2" sqref="B2 B15 B28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="4" max="4" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2512,7 +2513,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2523,7 +2524,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2540,7 +2541,7 @@
         <v>0.58278641200000003</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2557,7 +2558,7 @@
         <v>0.86286327206249125</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2580,7 +2581,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2598,7 +2599,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2615,7 +2616,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -2632,7 +2633,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2683,7 +2684,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2700,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -2710,7 +2711,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2731,7 +2732,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2746,7 +2747,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2767,7 +2768,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -2784,7 +2785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -2818,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -2835,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -2852,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -2886,7 +2887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -2907,7 +2908,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -2928,7 +2929,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -2938,7 +2939,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -2959,7 +2960,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -2970,7 +2971,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2987,7 +2988,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -3022,7 +3023,7 @@
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -3040,7 +3041,7 @@
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -3057,7 +3058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -3074,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -3091,7 +3092,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -3108,7 +3109,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -3125,7 +3126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -3142,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -3154,16 +3155,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -3180,7 +3181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3190,7 +3191,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -3204,7 +3205,7 @@
       </c>
       <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3236,7 +3237,7 @@
         <v>0.14669242738933452</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3268,7 +3269,7 @@
         <v>6.5822905632346718E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -3300,7 +3301,7 @@
         <v>0.19901892500000001</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3332,7 +3333,7 @@
         <v>2.5903149293944883E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -3364,7 +3365,7 @@
         <v>0.59454384808304517</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C8" s="2"/>
       <c r="D8" s="6"/>
       <c r="E8" s="2"/>
@@ -3377,7 +3378,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3393,7 +3394,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3415,7 +3416,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -3449,7 +3450,7 @@
       </c>
       <c r="S11" s="2"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3482,7 +3483,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -3514,7 +3515,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -3547,7 +3548,7 @@
         <v>0.72330960628535357</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -3579,13 +3580,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -3602,7 +3603,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -3634,7 +3635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3667,7 +3668,7 @@
       </c>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3699,7 +3700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>0.84690702284591701</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3763,16 +3764,16 @@
       </c>
       <c r="Q23" s="2"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="O28" s="2"/>
     </row>
-    <row r="41" spans="3:3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" s="9" t="str">
         <f>C3 &amp; "  " &amp; "(" &amp; D3 &amp; ")"</f>
         <v>415  (0.043312574)</v>

</xml_diff>

<commit_message>
added garch results jpmp
</commit_message>
<xml_diff>
--- a/Results/seminar_results.xlsx
+++ b/Results/seminar_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thani\Dropbox\R\Github\Quant-Finance-Seminar\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403ECB84-421E-46E2-9464-12157B653B60}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C240BCD3-D6F8-402A-85D6-9F5420D86073}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sp" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="h_day" sheetId="6" r:id="rId5"/>
     <sheet name="jpm" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="28">
   <si>
     <t>Cond. GARCH EVT</t>
   </si>
@@ -2463,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3137,8 +3137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -3186,6 +3186,9 @@
         <v>539</v>
       </c>
       <c r="M2" s="2"/>
+      <c r="O2" s="2">
+        <v>430</v>
+      </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
@@ -3217,6 +3220,12 @@
       </c>
       <c r="M3" s="6">
         <v>0.14669242738933452</v>
+      </c>
+      <c r="O3">
+        <v>305</v>
+      </c>
+      <c r="P3">
+        <v>0.71728347276289961</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -3410,7 +3419,9 @@
       <c r="L10" s="2">
         <v>108</v>
       </c>
-      <c r="O10" s="2"/>
+      <c r="O10" s="2">
+        <v>86</v>
+      </c>
       <c r="P10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -3448,8 +3459,12 @@
       <c r="M11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="O11">
+        <v>45</v>
+      </c>
+      <c r="P11">
+        <v>0.23882912235117201</v>
+      </c>
       <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:21">
@@ -3622,7 +3637,9 @@
       <c r="L18" s="2">
         <v>54</v>
       </c>
-      <c r="O18" s="2"/>
+      <c r="O18" s="2">
+        <v>43</v>
+      </c>
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:20">
@@ -3656,8 +3673,12 @@
       <c r="M19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+      <c r="O19">
+        <v>23</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
@@ -3819,8 +3840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280EEFA1-21EF-4B85-8479-2AEFA6236963}">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3862,10 +3883,18 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="B3">
+        <v>442</v>
+      </c>
+      <c r="C3">
+        <v>0.55110011069360265</v>
+      </c>
+      <c r="D3">
+        <v>1.9284213461172817E-2</v>
+      </c>
+      <c r="E3">
+        <v>5.4179451723915473E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
@@ -4014,6 +4043,18 @@
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B16">
+        <v>94</v>
+      </c>
+      <c r="C16">
+        <v>0.39177939898649916</v>
+      </c>
+      <c r="D16">
+        <v>4.138540289418402E-3</v>
+      </c>
+      <c r="E16">
+        <v>1.135940071649888E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
@@ -4142,10 +4183,18 @@
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="B29">
+        <v>52</v>
+      </c>
+      <c r="C29">
+        <v>0.18236853408949238</v>
+      </c>
+      <c r="D29">
+        <v>4.1884974491982252E-2</v>
+      </c>
+      <c r="E29">
+        <v>5.1869146460323035E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">

</xml_diff>